<commit_message>
add new exercises, section, update anki deck/wordlist
- updated anki deck/wordlist for Lesson 19. (3rd ed.)
- added new section for Lesson 20. (3rd ed.)
- added the following exercises.

# Lesson 19 (3rd ed.)
- Reading Practice: マリアさんのメール
- Useful Expressions: Greeting Cards
- Workbook: Kanji Writing Practice
- Workbook: Using Kanji
</commit_message>
<xml_diff>
--- a/resources/tools/wordlist_E-J/lessons-3rd/lesson-19.xlsx
+++ b/resources/tools/wordlist_E-J/lessons-3rd/lesson-19.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B110"/>
+  <dimension ref="A1:B119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1048,694 +1048,802 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>Happy New Year</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>春|はる</t>
+          <t>あけましておめでとうございます</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>spring roll</t>
+          <t>Happy New Year (kanji)</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>春巻|はるまき</t>
+          <t>謹賀新年|きんがしんねん</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>vernal equinox</t>
+          <t>Thank you for all your kind help during the past year.</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>春分|しゅんぶん</t>
+          <t>昨年は大変お世話になりました|さくねんはたいへんおせわになりました</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>youth</t>
+          <t>I hope for your continued good will this year.</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>青春|せいしゅん</t>
+          <t>本年もどうぞよろしくお願いいたします|ほんねんもどうぞよろしくおねがいいたします</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>I hope you are keeping well during the hot weather.</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>秋|あき</t>
+          <t>暑中お見舞い申し上げます|しょちゅうおみまいもうしあげます</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>fall semester</t>
+          <t>Congratulations on your graduation.</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>秋学期|あきがっき</t>
+          <t>ご卒業おめでとうございます|ごそつぎょうおめでとうございます</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>autumnal equinox</t>
+          <t>Congratulations on your marriage.</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>秋分|しゅうぶん</t>
+          <t>ご結婚おめでとうございます|ごけっこんおめでとうございます</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>winter</t>
+          <t>Happy Birthday</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>冬|ふゆ</t>
+          <t>誕生日おめでとう|たんじょうびおめでとう</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>winter vacation</t>
+          <t>Get well soon.</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>冬休み|ふゆやすみ</t>
+          <t>早くよくなってください|はやくよくなってください</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>warm winter</t>
+          <t>spring</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>暖冬|だんとう</t>
+          <t>春|はる</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>four seasons</t>
+          <t>spring roll</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>春夏秋冬|しゅんかしゅうとう</t>
+          <t>春巻|はるまき</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>flower</t>
+          <t>vernal equinox</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>花|はな</t>
+          <t>春分|しゅんぶん</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>flower viewing</t>
+          <t>youth</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>花見|はなみ</t>
+          <t>青春|せいしゅん</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>fireworks</t>
+          <t>autumn</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>花火|はなび</t>
+          <t>秋|あき</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>hay fever</t>
+          <t>fall semester</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>花粉症|かふんしょう</t>
+          <t>秋学期|あきがっき</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>flower arrangement</t>
+          <t>autumnal equinox</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>生け花|いけばな</t>
+          <t>秋分|しゅうぶん</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Mr./Ms.</t>
+          <t>winter</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>～様|～さま</t>
+          <t>冬|ふゆ</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>customer (respectful)</t>
+          <t>winter vacation</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>お客様|おきゃくさま</t>
+          <t>冬休み|ふゆやすみ</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>everyone</t>
+          <t>warm winter</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>皆様|みなさま</t>
+          <t>暖冬|だんとう</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>manner</t>
+          <t>four seasons</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>様子|ようす</t>
+          <t>春夏秋冬|しゅんかしゅうとう</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>uneasy; worried</t>
+          <t>flower</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>不安な|ふあんな</t>
+          <t>花|はな</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>recession</t>
+          <t>flower viewing</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>不景気|ふけいき</t>
+          <t>花見|はなみ</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>inconvenience</t>
+          <t>fireworks</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>不便|ふべん</t>
+          <t>花火|はなび</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>lack of water</t>
+          <t>hay fever</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>水不足|みずぶそく</t>
+          <t>花粉症|かふんしょう</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>older sister</t>
+          <t>flower arrangement</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>姉|あね</t>
+          <t>生け花|いけばな</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>older sister (honorific)</t>
+          <t>Mr./Ms.</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>お姉さん|おねえさん</t>
+          <t>～様|～さま</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>sisters</t>
+          <t>customer (respectful)</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>姉妹|しまい</t>
+          <t>お客様|おきゃくさま</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>sister city</t>
+          <t>everyone</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>姉妹都市|しまいとし</t>
+          <t>皆様|みなさま</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>older brother</t>
+          <t>manner</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>兄|あに</t>
+          <t>様子|ようす</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>older brother (honorific)</t>
+          <t>uneasy; worried</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>お兄さん|おにいさん</t>
+          <t>不安な|ふあんな</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>brothers</t>
+          <t>recession</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>兄弟|きょうだい</t>
+          <t>不景気|ふけいき</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Chinese character</t>
+          <t>inconvenience</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>漢字|かんじ</t>
+          <t>不便|ふべん</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Chinese herbal medicine</t>
+          <t>lack of water</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>漢方薬|かんぽうやく</t>
+          <t>水不足|みずぶそく</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Kanji dictionary</t>
+          <t>older sister</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>漢和辞典|かんわじてん</t>
+          <t>姉|あね</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>to graduate</t>
+          <t>older sister (honorific)</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>卒業する|そつぎょうする</t>
+          <t>お姉さん|おねえさん</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>graduation ceremony</t>
+          <t>sisters</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>卒業式|そつぎょうしき</t>
+          <t>姉妹|しまい</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>university graduate</t>
+          <t>sister city</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>大卒|だいそつ</t>
+          <t>姉妹都市|しまいとし</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>engineering</t>
+          <t>older brother</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>工学|こうがく</t>
+          <t>兄|あに</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>construction</t>
+          <t>older brother (honorific)</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>工事|こうじ</t>
+          <t>お兄さん|おにいさん</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>factory</t>
+          <t>brothers</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>工場|こうじょう</t>
+          <t>兄弟|きょうだい</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>carpenter</t>
+          <t>Chinese character</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>大工|だいく</t>
+          <t>漢字|かんじ</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>research</t>
+          <t>Chinese herbal medicine</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>研究|けんきゅう</t>
+          <t>漢方薬|かんぽうやく</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>researcher</t>
+          <t>Kanji dictionary</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>研究者|けんきゅうしゃ</t>
+          <t>漢和辞典|かんわじてん</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>training</t>
+          <t>to graduate</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>研修|けんしゅう</t>
+          <t>卒業する|そつぎょうする</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>to sharpen</t>
+          <t>graduation ceremony</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>研ぐ|とぐ</t>
+          <t>卒業式|そつぎょうしき</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>inquiry</t>
+          <t>university graduate</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>探究|たんきゅう</t>
+          <t>大卒|だいそつ</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>to investigate thoroughly</t>
+          <t>engineering</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>究める|きわめる</t>
+          <t>工学|こうがく</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>question</t>
+          <t>construction</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>質問|しつもん</t>
+          <t>工事|こうじ</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>good quality</t>
+          <t>factory</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>質がいい|しつがいい</t>
+          <t>工場|こうじょう</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>aptitude</t>
+          <t>carpenter</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>素質|そしつ</t>
+          <t>大工|だいく</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>pawn shop</t>
+          <t>research</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>質屋|しちや</t>
+          <t>研究|けんきゅう</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>problem</t>
+          <t>researcher</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>問題|もんだい</t>
+          <t>研究者|けんきゅうしゃ</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>visit</t>
+          <t>training</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>訪問|ほうもん</t>
+          <t>研修|けんしゅう</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>to question</t>
+          <t>to sharpen</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>問う|とう</t>
+          <t>研ぐ|とぐ</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>many</t>
+          <t>inquiry</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>多い|おおい</t>
+          <t>探究|たんきゅう</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>probably</t>
+          <t>to investigate thoroughly</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>多分|たぶん</t>
+          <t>究める|きわめる</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>many of...</t>
+          <t>question</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>～の多く|～のおおく</t>
+          <t>質問|しつもん</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
+          <t>good quality</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>質がいい|しつがいい</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>aptitude</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>素質|そしつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>pawn shop</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>質屋|しちや</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>problem</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>問題|もんだい</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>visit</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>訪問|ほうもん</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>to question</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>問う|とう</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>many</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>多い|おおい</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>probably</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>多分|たぶん</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>many of...</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>～の多く|～のおおく</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
           <t>decision by majority</t>
         </is>
       </c>
-      <c r="B110" t="inlineStr">
+      <c r="B119" t="inlineStr">
         <is>
           <t>多数決|たすうけつ</t>
         </is>

</xml_diff>